<commit_message>
Time delay and lag 2 disturbance rejection
</commit_message>
<xml_diff>
--- a/Benchmark_System/Time Delay and Lag 2/Time Delay and Lag2_dist.xlsx
+++ b/Benchmark_System/Time Delay and Lag 2/Time Delay and Lag2_dist.xlsx
@@ -138,10 +138,10 @@
         <v>1</v>
       </c>
       <c r="B2">
-        <v>0.6272061584496893</v>
+        <v>0.63572591109317322</v>
       </c>
       <c r="C2">
-        <v>0.62856846795117993</v>
+        <v>0.59358603128570442</v>
       </c>
     </row>
     <row r="3">
@@ -149,10 +149,10 @@
         <v>2</v>
       </c>
       <c r="B3">
-        <v>2.7161627021596031</v>
+        <v>2.6783732504971551</v>
       </c>
       <c r="C3">
-        <v>2.6261179758637425</v>
+        <v>2.9989071078059713</v>
       </c>
     </row>
     <row r="4">
@@ -160,10 +160,10 @@
         <v>3</v>
       </c>
       <c r="B4">
-        <v>1.3760235346289835</v>
+        <v>1.3921530470386705</v>
       </c>
       <c r="C4">
-        <v>1.3117365816809108</v>
+        <v>1.6419451794316096</v>
       </c>
     </row>
     <row r="5">
@@ -171,10 +171,10 @@
         <v>4</v>
       </c>
       <c r="B5">
-        <v>0.45453526169391339</v>
+        <v>0.44525456386918649</v>
       </c>
       <c r="C5">
-        <v>0.47533233774667155</v>
+        <v>0.32797522362799547</v>
       </c>
     </row>
     <row r="6">
@@ -182,7 +182,7 @@
         <v>5</v>
       </c>
       <c r="C6">
-        <v>2.7645188106289047</v>
+        <v>0.10241660106831009</v>
       </c>
     </row>
     <row r="7">
@@ -212,10 +212,10 @@
         <v>8</v>
       </c>
       <c r="B9">
-        <v>4545.3526169391334</v>
+        <v>52.774295247091352</v>
       </c>
       <c r="C9">
-        <v>4753.3233774667151</v>
+        <v>1.7852239589195316</v>
       </c>
     </row>
     <row r="10">
@@ -223,7 +223,7 @@
         <v>9</v>
       </c>
       <c r="C10">
-        <v>0.30513829441431317</v>
+        <v>0.763852963893773</v>
       </c>
     </row>
     <row r="11">
@@ -242,10 +242,10 @@
         <v>11</v>
       </c>
       <c r="B12">
-        <v>6.9979982553042648</v>
+        <v>7.0696844086353581</v>
       </c>
       <c r="C12">
-        <v>7.0032603973249881</v>
+        <v>7.1894752448428525</v>
       </c>
     </row>
     <row r="13">
@@ -275,10 +275,10 @@
         <v>14</v>
       </c>
       <c r="B15">
-        <v>0.39323733130280425</v>
+        <v>0.39532975386303709</v>
       </c>
       <c r="C15">
-        <v>0.39306571179747907</v>
+        <v>0.40237362005736332</v>
       </c>
     </row>
     <row r="16">
@@ -286,10 +286,10 @@
         <v>15</v>
       </c>
       <c r="B16">
-        <v>2.0039156139041601</v>
+        <v>2.0184628303544039</v>
       </c>
       <c r="C16">
-        <v>2.0116914053755113</v>
+        <v>2.0633518837148306</v>
       </c>
     </row>
   </sheetData>

</xml_diff>